<commit_message>
Attempted Bold, Italic, Underline Functionality
Hopefully this comes out as a fork. Or branch. Still unfamiliar with terminology.  This push is not functional, hence I do not want to override the master branch.
</commit_message>
<xml_diff>
--- a/Writer's Block/ProgressSheet.xlsx
+++ b/Writer's Block/ProgressSheet.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Completed</t>
-  </si>
-  <si>
     <t>Completed By</t>
   </si>
   <si>
@@ -39,7 +36,19 @@
     <t>Learned/Practiced</t>
   </si>
   <si>
-    <t>Jquery. GIT pushing. Manipulating the DOM with JS. CSS stylzing and element hierachy. HTML Elements.</t>
+    <t>Jquery. GIT pushing. Manipulating the DOM with JS. CSS stylzing and element hierarchy. HTML Elements.</t>
+  </si>
+  <si>
+    <t>To Do</t>
+  </si>
+  <si>
+    <t>Completed / Log</t>
+  </si>
+  <si>
+    <t>Added "bold," "italic," and "underline" buttons. Do not function properly yet. Researched File Uploading in Jquery.</t>
+  </si>
+  <si>
+    <t>Manipulating text in textarea to be bold, italic, or underlined. Options for Jquery file upload. AJAX seems like the best option, it updates files on to the server, but without having to render the page again. Called a dynamic process - manipulates the DOM. There are also plugins for File Uploading that are available.   Created a fork in GITHub.</t>
   </si>
 </sst>
 </file>
@@ -88,10 +97,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -395,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,24 +416,24 @@
     <col min="2" max="2" width="108.5703125" customWidth="1"/>
     <col min="3" max="3" width="38.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="100.5703125" customWidth="1"/>
+    <col min="5" max="5" width="121.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -432,15 +441,37 @@
         <v>42882</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42883</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>